<commit_message>
completed verse 14, started verse 15
</commit_message>
<xml_diff>
--- a/ref/Bible_data_ch_verses.xlsx
+++ b/ref/Bible_data_ch_verses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0CFE8903-B752-4CD1-A1C7-3C8DA6A8589B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E1D8687-9DEB-4F0F-B34F-C885F69FEDD3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1101,7 +1101,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K33" sqref="K33"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,13 +1151,13 @@
       <c r="L1" s="3">
         <v>11</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M1" s="3">
         <v>12</v>
       </c>
-      <c r="N1" s="1">
+      <c r="N1" s="3">
         <v>13</v>
       </c>
-      <c r="O1" s="1">
+      <c r="O1" s="5">
         <v>14</v>
       </c>
       <c r="P1" s="1">
@@ -1891,7 +1891,7 @@
       <c r="AJ5">
         <v>34</v>
       </c>
-      <c r="AK5">
+      <c r="AK5" s="2">
         <v>13</v>
       </c>
       <c r="AL5" t="s">
@@ -2040,7 +2040,7 @@
       <c r="AH6">
         <v>29</v>
       </c>
-      <c r="AI6" s="6">
+      <c r="AI6" s="2">
         <v>12</v>
       </c>
       <c r="AJ6" t="s">
@@ -2263,7 +2263,7 @@
       <c r="Q8">
         <v>31</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="2">
         <v>13</v>
       </c>
       <c r="S8">
@@ -2396,7 +2396,7 @@
       <c r="E10">
         <v>22</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="2">
         <v>12</v>
       </c>
       <c r="G10">
@@ -2462,7 +2462,7 @@
       <c r="AA10">
         <v>25</v>
       </c>
-      <c r="AB10" s="6">
+      <c r="AB10" s="2">
         <v>12</v>
       </c>
       <c r="AC10">
@@ -2474,7 +2474,7 @@
       <c r="AE10">
         <v>31</v>
       </c>
-      <c r="AF10">
+      <c r="AF10" s="2">
         <v>13</v>
       </c>
       <c r="AL10" t="s">
@@ -2533,7 +2533,7 @@
       <c r="D11">
         <v>39</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="2">
         <v>12</v>
       </c>
       <c r="F11">
@@ -2548,7 +2548,7 @@
       <c r="I11">
         <v>18</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="2">
         <v>13</v>
       </c>
       <c r="K11">
@@ -2905,7 +2905,7 @@
       <c r="J14">
         <v>44</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="6">
         <v>14</v>
       </c>
       <c r="L14">
@@ -2914,7 +2914,7 @@
       <c r="M14">
         <v>41</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="6">
         <v>14</v>
       </c>
       <c r="O14">
@@ -3024,7 +3024,7 @@
       <c r="E15">
         <v>22</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>14</v>
       </c>
       <c r="G15">
@@ -3051,13 +3051,13 @@
       <c r="N15">
         <v>23</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="6">
         <v>14</v>
       </c>
       <c r="P15">
         <v>19</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="6">
         <v>14</v>
       </c>
       <c r="R15">
@@ -3075,7 +3075,7 @@
       <c r="V15">
         <v>20</v>
       </c>
-      <c r="W15" s="6">
+      <c r="W15" s="2">
         <v>12</v>
       </c>
       <c r="X15">
@@ -3173,7 +3173,7 @@
       <c r="C16">
         <v>70</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>13</v>
       </c>
       <c r="E16">
@@ -3342,10 +3342,10 @@
       <c r="E18">
         <v>17</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>14</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>14</v>
       </c>
       <c r="H18" s="2">
@@ -3428,7 +3428,7 @@
       <c r="B19">
         <v>22</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>13</v>
       </c>
       <c r="D19">
@@ -3500,7 +3500,7 @@
       <c r="Z19">
         <v>6</v>
       </c>
-      <c r="AA19">
+      <c r="AA19" s="6">
         <v>14</v>
       </c>
       <c r="AB19">
@@ -3568,7 +3568,7 @@
       <c r="E20" s="2">
         <v>9</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>13</v>
       </c>
       <c r="G20" s="2">
@@ -3616,7 +3616,7 @@
       <c r="U20" s="4">
         <v>10</v>
       </c>
-      <c r="V20">
+      <c r="V20" s="6">
         <v>14</v>
       </c>
       <c r="W20">
@@ -3634,7 +3634,7 @@
       <c r="AA20" s="2">
         <v>11</v>
       </c>
-      <c r="AB20">
+      <c r="AB20" s="6">
         <v>14</v>
       </c>
       <c r="AC20" s="2">
@@ -3643,7 +3643,7 @@
       <c r="AD20" s="2">
         <v>11</v>
       </c>
-      <c r="AE20">
+      <c r="AE20" s="2">
         <v>13</v>
       </c>
       <c r="AF20">
@@ -3661,7 +3661,7 @@
       <c r="AJ20">
         <v>28</v>
       </c>
-      <c r="AK20">
+      <c r="AK20" s="2">
         <v>13</v>
       </c>
       <c r="AL20">
@@ -3670,16 +3670,16 @@
       <c r="AM20">
         <v>23</v>
       </c>
-      <c r="AN20">
+      <c r="AN20" s="6">
         <v>14</v>
       </c>
       <c r="AO20">
         <v>18</v>
       </c>
-      <c r="AP20">
+      <c r="AP20" s="6">
         <v>14</v>
       </c>
-      <c r="AQ20" s="6">
+      <c r="AQ20" s="2">
         <v>12</v>
       </c>
       <c r="AR20">
@@ -3691,7 +3691,7 @@
       <c r="AT20">
         <v>18</v>
       </c>
-      <c r="AU20" s="6">
+      <c r="AU20" s="2">
         <v>12</v>
       </c>
       <c r="AV20" s="2">
@@ -3726,34 +3726,34 @@
       <c r="F21">
         <v>24</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="6">
         <v>14</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="2">
         <v>12</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="2">
         <v>12</v>
       </c>
       <c r="J21">
         <v>18</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="6">
         <v>14</v>
       </c>
       <c r="L21" s="2">
         <v>9</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="2">
         <v>13</v>
       </c>
-      <c r="N21" s="6">
+      <c r="N21" s="2">
         <v>12</v>
       </c>
       <c r="O21" s="2">
         <v>11</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="6">
         <v>14</v>
       </c>
       <c r="Q21">
@@ -3786,7 +3786,7 @@
       <c r="Z21" s="2">
         <v>11</v>
       </c>
-      <c r="AA21">
+      <c r="AA21" s="2">
         <v>13</v>
       </c>
       <c r="AB21">
@@ -3795,7 +3795,7 @@
       <c r="AC21">
         <v>72</v>
       </c>
-      <c r="AD21">
+      <c r="AD21" s="2">
         <v>13</v>
       </c>
       <c r="AE21">
@@ -3810,10 +3810,10 @@
       <c r="AH21">
         <v>19</v>
       </c>
-      <c r="AI21">
+      <c r="AI21" s="2">
         <v>13</v>
       </c>
-      <c r="AJ21">
+      <c r="AJ21" s="6">
         <v>14</v>
       </c>
       <c r="AK21">
@@ -3846,10 +3846,10 @@
       <c r="AT21" s="2">
         <v>11</v>
       </c>
-      <c r="AU21">
+      <c r="AU21" s="2">
         <v>13</v>
       </c>
-      <c r="AV21" s="6">
+      <c r="AV21" s="2">
         <v>12</v>
       </c>
       <c r="AW21" s="2">
@@ -3887,7 +3887,7 @@
       <c r="H22">
         <v>43</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="6">
         <v>14</v>
       </c>
       <c r="J22">
@@ -3983,7 +3983,7 @@
       <c r="AN22">
         <v>24</v>
       </c>
-      <c r="AO22">
+      <c r="AO22" s="6">
         <v>14</v>
       </c>
       <c r="AP22" s="2">
@@ -3992,7 +3992,7 @@
       <c r="AQ22">
         <v>8</v>
       </c>
-      <c r="AR22" s="6">
+      <c r="AR22" s="2">
         <v>12</v>
       </c>
       <c r="AS22">
@@ -4007,7 +4007,7 @@
       <c r="AV22">
         <v>20</v>
       </c>
-      <c r="AW22">
+      <c r="AW22" s="6">
         <v>14</v>
       </c>
       <c r="AX22" s="2">
@@ -4134,7 +4134,7 @@
       <c r="F24">
         <v>19</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="2">
         <v>12</v>
       </c>
       <c r="H24">
@@ -4152,7 +4152,7 @@
       <c r="L24" s="2">
         <v>10</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="6">
         <v>14</v>
       </c>
     </row>
@@ -4175,13 +4175,13 @@
       <c r="F25">
         <v>16</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="2">
         <v>12</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="6">
         <v>14</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="6">
         <v>14</v>
       </c>
     </row>
@@ -4204,7 +4204,7 @@
       <c r="F26">
         <v>30</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <v>13</v>
       </c>
       <c r="H26">
@@ -4234,10 +4234,10 @@
       <c r="P26" s="2">
         <v>9</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="6">
         <v>14</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="6">
         <v>14</v>
       </c>
       <c r="S26">
@@ -4261,13 +4261,13 @@
       <c r="Y26">
         <v>23</v>
       </c>
-      <c r="Z26" s="6">
+      <c r="Z26" s="2">
         <v>12</v>
       </c>
       <c r="AA26">
         <v>21</v>
       </c>
-      <c r="AB26">
+      <c r="AB26" s="2">
         <v>13</v>
       </c>
       <c r="AC26">
@@ -4324,7 +4324,7 @@
       <c r="AT26">
         <v>25</v>
       </c>
-      <c r="AU26">
+      <c r="AU26" s="2">
         <v>13</v>
       </c>
       <c r="AV26">
@@ -4345,22 +4345,22 @@
       <c r="BA26">
         <v>15</v>
       </c>
-      <c r="BB26" s="6">
+      <c r="BB26" s="2">
         <v>12</v>
       </c>
       <c r="BC26">
         <v>17</v>
       </c>
-      <c r="BD26">
+      <c r="BD26" s="2">
         <v>13</v>
       </c>
-      <c r="BE26" s="6">
+      <c r="BE26" s="2">
         <v>12</v>
       </c>
       <c r="BF26">
         <v>21</v>
       </c>
-      <c r="BG26">
+      <c r="BG26" s="6">
         <v>14</v>
       </c>
       <c r="BH26">
@@ -4372,7 +4372,7 @@
       <c r="BJ26" s="2">
         <v>11</v>
       </c>
-      <c r="BK26" s="6">
+      <c r="BK26" s="2">
         <v>12</v>
       </c>
       <c r="BL26">
@@ -4452,7 +4452,7 @@
       <c r="U27">
         <v>18</v>
       </c>
-      <c r="V27">
+      <c r="V27" s="6">
         <v>14</v>
       </c>
       <c r="W27">
@@ -4518,7 +4518,7 @@
       <c r="AQ27">
         <v>22</v>
       </c>
-      <c r="AR27">
+      <c r="AR27" s="2">
         <v>13</v>
       </c>
       <c r="AS27">
@@ -4588,7 +4588,7 @@
       <c r="F29">
         <v>17</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="6">
         <v>14</v>
       </c>
       <c r="H29">
@@ -4627,7 +4627,7 @@
       <c r="S29">
         <v>32</v>
       </c>
-      <c r="T29">
+      <c r="T29" s="6">
         <v>14</v>
       </c>
       <c r="U29">
@@ -4755,7 +4755,7 @@
       <c r="L30">
         <v>45</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="2">
         <v>13</v>
       </c>
       <c r="N30">
@@ -4790,7 +4790,7 @@
       <c r="H31">
         <v>16</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="6">
         <v>14</v>
       </c>
       <c r="J31">
@@ -4842,19 +4842,19 @@
       <c r="D33">
         <v>15</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>13</v>
       </c>
       <c r="F33">
         <v>27</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="6">
         <v>14</v>
       </c>
       <c r="H33">
         <v>17</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="6">
         <v>14</v>
       </c>
       <c r="J33">
@@ -4893,16 +4893,16 @@
       <c r="B36">
         <v>16</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>13</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="2">
         <v>12</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>14</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>14</v>
       </c>
       <c r="G36">
@@ -4916,10 +4916,10 @@
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <v>14</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>14</v>
       </c>
       <c r="D37">
@@ -4978,7 +4978,7 @@
       <c r="D41" s="2">
         <v>10</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>14</v>
       </c>
       <c r="F41" s="2">
@@ -4987,7 +4987,7 @@
       <c r="G41">
         <v>15</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="6">
         <v>14</v>
       </c>
       <c r="I41">
@@ -4996,13 +4996,13 @@
       <c r="J41">
         <v>17</v>
       </c>
-      <c r="K41" s="6">
+      <c r="K41" s="2">
         <v>12</v>
       </c>
       <c r="L41">
         <v>17</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="6">
         <v>14</v>
       </c>
       <c r="N41" s="2">
@@ -5016,7 +5016,7 @@
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="2">
         <v>14</v>
       </c>
       <c r="C42">
@@ -5442,7 +5442,7 @@
       <c r="M48">
         <v>21</v>
       </c>
-      <c r="N48">
+      <c r="N48" s="6">
         <v>14</v>
       </c>
       <c r="O48">
@@ -5471,7 +5471,7 @@
       <c r="E49">
         <v>21</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="2">
         <v>13</v>
       </c>
       <c r="G49">
@@ -5480,7 +5480,7 @@
       <c r="H49">
         <v>40</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="2">
         <v>13</v>
       </c>
       <c r="J49">
@@ -5495,7 +5495,7 @@
       <c r="M49">
         <v>31</v>
       </c>
-      <c r="N49">
+      <c r="N49" s="2">
         <v>13</v>
       </c>
       <c r="O49">
@@ -5548,7 +5548,7 @@
       <c r="M50">
         <v>21</v>
       </c>
-      <c r="N50">
+      <c r="N50" s="2">
         <v>13</v>
       </c>
     </row>
@@ -5642,7 +5642,7 @@
       <c r="C55">
         <v>20</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="2">
         <v>13</v>
       </c>
       <c r="E55">
@@ -5656,7 +5656,7 @@
       <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="2">
         <v>12</v>
       </c>
       <c r="C56">
@@ -5732,7 +5732,7 @@
       <c r="A61" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="2">
         <v>14</v>
       </c>
       <c r="C61">
@@ -5744,7 +5744,7 @@
       <c r="E61">
         <v>16</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="2">
         <v>14</v>
       </c>
       <c r="G61">
@@ -5753,7 +5753,7 @@
       <c r="H61">
         <v>28</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="2">
         <v>13</v>
       </c>
       <c r="J61">
@@ -5788,7 +5788,7 @@
       <c r="E62">
         <v>17</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="2">
         <v>20</v>
       </c>
     </row>
@@ -5808,7 +5808,7 @@
       <c r="E63">
         <v>19</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="2">
         <v>14</v>
       </c>
     </row>
@@ -5825,6 +5825,7 @@
       <c r="D64">
         <v>18</v>
       </c>
+      <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
@@ -5842,7 +5843,7 @@
       <c r="E65">
         <v>21</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="2">
         <v>21</v>
       </c>
     </row>
@@ -5850,9 +5851,10 @@
       <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="2">
         <v>13</v>
       </c>
+      <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
@@ -5861,6 +5863,7 @@
       <c r="B67">
         <v>15</v>
       </c>
+      <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -5869,6 +5872,7 @@
       <c r="B68">
         <v>25</v>
       </c>
+      <c r="F68" s="2"/>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
@@ -5886,7 +5890,7 @@
       <c r="E69" s="2">
         <v>11</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="2">
         <v>14</v>
       </c>
       <c r="G69">
@@ -5895,7 +5899,7 @@
       <c r="H69">
         <v>17</v>
       </c>
-      <c r="I69">
+      <c r="I69" s="2">
         <v>13</v>
       </c>
       <c r="J69">

</xml_diff>

<commit_message>
finished verses 16 - 22
</commit_message>
<xml_diff>
--- a/ref/Bible_data_ch_verses.xlsx
+++ b/ref/Bible_data_ch_verses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DCFD6655-F171-42F2-B2E1-BB9DBDD2BFF3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{43A11AB3-F650-4E44-8A25-4A32D79062DE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,45 +169,9 @@
     <t>Rom</t>
   </si>
   <si>
-    <t>1 Cor</t>
-  </si>
-  <si>
-    <t>2 Cor</t>
-  </si>
-  <si>
-    <t>Gal</t>
-  </si>
-  <si>
-    <t>Eph</t>
-  </si>
-  <si>
-    <t>Phil</t>
-  </si>
-  <si>
-    <t>Col</t>
-  </si>
-  <si>
-    <t>1Thess</t>
-  </si>
-  <si>
-    <t>2Thess</t>
-  </si>
-  <si>
-    <t>1 Tim</t>
-  </si>
-  <si>
-    <t>2 Tim</t>
-  </si>
-  <si>
     <t>Titus</t>
   </si>
   <si>
-    <t>Phlm</t>
-  </si>
-  <si>
-    <t>Heb</t>
-  </si>
-  <si>
     <t>James</t>
   </si>
   <si>
@@ -229,7 +193,43 @@
     <t>Jude</t>
   </si>
   <si>
-    <t>Rev</t>
+    <t>Ephesians</t>
+  </si>
+  <si>
+    <t>Philippians</t>
+  </si>
+  <si>
+    <t>Colossians</t>
+  </si>
+  <si>
+    <t>1 Corinthians</t>
+  </si>
+  <si>
+    <t>2 Corinthians</t>
+  </si>
+  <si>
+    <t>1 Thessalonians</t>
+  </si>
+  <si>
+    <t>2 Thessalonians</t>
+  </si>
+  <si>
+    <t>1 Timothy</t>
+  </si>
+  <si>
+    <t>2 Timothy</t>
+  </si>
+  <si>
+    <t>Phileman</t>
+  </si>
+  <si>
+    <t>Hebrews</t>
+  </si>
+  <si>
+    <t>Revelation</t>
+  </si>
+  <si>
+    <t>Galatians</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1093,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD13" sqref="AD13"/>
+      <selection pane="bottomRight" activeCell="AT22" sqref="AT22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,25 +1152,25 @@
       <c r="O1" s="3">
         <v>14</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P1" s="3">
         <v>15</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="Q1" s="3">
         <v>16</v>
       </c>
-      <c r="R1" s="1">
+      <c r="R1" s="3">
         <v>17</v>
       </c>
-      <c r="S1" s="1">
+      <c r="S1" s="3">
         <v>18</v>
       </c>
-      <c r="T1" s="1">
+      <c r="T1" s="3">
         <v>19</v>
       </c>
-      <c r="U1" s="1">
+      <c r="U1" s="3">
         <v>20</v>
       </c>
-      <c r="V1" s="1">
+      <c r="V1" s="3">
         <v>21</v>
       </c>
       <c r="W1" s="1">
@@ -1346,19 +1346,19 @@
       <c r="L2">
         <v>32</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="2">
         <v>20</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="2">
         <v>18</v>
       </c>
       <c r="O2">
         <v>24</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="2">
         <v>21</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="2">
         <v>16</v>
       </c>
       <c r="R2">
@@ -1370,7 +1370,7 @@
       <c r="T2">
         <v>38</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="2">
         <v>18</v>
       </c>
       <c r="V2">
@@ -1379,7 +1379,7 @@
       <c r="W2">
         <v>24</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="2">
         <v>20</v>
       </c>
       <c r="Y2">
@@ -1409,7 +1409,7 @@
       <c r="AG2">
         <v>33</v>
       </c>
-      <c r="AH2">
+      <c r="AH2" s="2">
         <v>20</v>
       </c>
       <c r="AI2">
@@ -1516,7 +1516,7 @@
       <c r="Q3">
         <v>36</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="2">
         <v>16</v>
       </c>
       <c r="S3">
@@ -1537,7 +1537,7 @@
       <c r="X3">
         <v>33</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="2">
         <v>18</v>
       </c>
       <c r="Z3">
@@ -1546,7 +1546,7 @@
       <c r="AA3">
         <v>37</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="2">
         <v>21</v>
       </c>
       <c r="AC3">
@@ -1558,7 +1558,7 @@
       <c r="AE3">
         <v>38</v>
       </c>
-      <c r="AF3">
+      <c r="AF3" s="2">
         <v>18</v>
       </c>
       <c r="AG3">
@@ -1623,13 +1623,13 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>17</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>16</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>17</v>
       </c>
       <c r="E4">
@@ -1650,7 +1650,7 @@
       <c r="J4">
         <v>24</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2">
         <v>20</v>
       </c>
       <c r="L4">
@@ -1671,7 +1671,7 @@
       <c r="Q4">
         <v>34</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="2">
         <v>16</v>
       </c>
       <c r="S4">
@@ -1811,7 +1811,7 @@
       <c r="L5">
         <v>35</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="2">
         <v>16</v>
       </c>
       <c r="N5">
@@ -1850,7 +1850,7 @@
       <c r="Y5">
         <v>25</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="2">
         <v>19</v>
       </c>
       <c r="AA5">
@@ -1865,7 +1865,7 @@
       <c r="AD5">
         <v>39</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="2">
         <v>17</v>
       </c>
       <c r="AF5">
@@ -1954,7 +1954,7 @@
       <c r="H6">
         <v>26</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <v>20</v>
       </c>
       <c r="J6">
@@ -1969,7 +1969,7 @@
       <c r="M6">
         <v>31</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="2">
         <v>19</v>
       </c>
       <c r="O6">
@@ -1981,16 +1981,16 @@
       <c r="Q6">
         <v>22</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="2">
         <v>20</v>
       </c>
       <c r="S6">
         <v>22</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="2">
         <v>21</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="2">
         <v>20</v>
       </c>
       <c r="V6">
@@ -2005,10 +2005,10 @@
       <c r="Y6">
         <v>22</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="2">
         <v>19</v>
       </c>
-      <c r="AA6">
+      <c r="AA6" s="2">
         <v>19</v>
       </c>
       <c r="AB6">
@@ -2020,7 +2020,7 @@
       <c r="AD6">
         <v>28</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="2">
         <v>20</v>
       </c>
       <c r="AF6">
@@ -2088,19 +2088,19 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>18</v>
       </c>
       <c r="C7">
         <v>24</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>17</v>
       </c>
       <c r="E7">
         <v>24</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>15</v>
       </c>
       <c r="G7">
@@ -2127,7 +2127,7 @@
       <c r="N7">
         <v>33</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="2">
         <v>15</v>
       </c>
       <c r="P7">
@@ -2136,7 +2136,7 @@
       <c r="Q7" s="2">
         <v>10</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="2">
         <v>18</v>
       </c>
       <c r="S7">
@@ -2154,7 +2154,7 @@
       <c r="W7">
         <v>34</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="2">
         <v>16</v>
       </c>
       <c r="Y7">
@@ -2234,22 +2234,22 @@
       <c r="J8">
         <v>57</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="2">
         <v>18</v>
       </c>
       <c r="L8">
         <v>40</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="2">
         <v>15</v>
       </c>
       <c r="N8">
         <v>25</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="2">
         <v>20</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="2">
         <v>20</v>
       </c>
       <c r="Q8">
@@ -2323,7 +2323,7 @@
       <c r="C9">
         <v>23</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>18</v>
       </c>
       <c r="E9">
@@ -2382,7 +2382,7 @@
       <c r="C10">
         <v>36</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>21</v>
       </c>
       <c r="E10">
@@ -2391,10 +2391,10 @@
       <c r="F10" s="2">
         <v>12</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>21</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>17</v>
       </c>
       <c r="I10">
@@ -2406,7 +2406,7 @@
       <c r="K10">
         <v>27</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="2">
         <v>15</v>
       </c>
       <c r="M10">
@@ -2436,7 +2436,7 @@
       <c r="U10">
         <v>42</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="2">
         <v>16</v>
       </c>
       <c r="W10">
@@ -2537,13 +2537,13 @@
       <c r="H11">
         <v>29</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>18</v>
       </c>
       <c r="J11" s="2">
         <v>13</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="2">
         <v>19</v>
       </c>
       <c r="L11">
@@ -2644,7 +2644,7 @@
       <c r="D12">
         <v>28</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>20</v>
       </c>
       <c r="F12">
@@ -2689,7 +2689,7 @@
       <c r="S12">
         <v>46</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="2">
         <v>21</v>
       </c>
       <c r="U12">
@@ -2748,7 +2748,7 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>18</v>
       </c>
       <c r="C13">
@@ -2766,7 +2766,7 @@
       <c r="G13">
         <v>33</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>20</v>
       </c>
       <c r="I13">
@@ -2778,7 +2778,7 @@
       <c r="K13">
         <v>36</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="2">
         <v>20</v>
       </c>
       <c r="M13">
@@ -2793,7 +2793,7 @@
       <c r="P13">
         <v>38</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="2">
         <v>20</v>
       </c>
       <c r="R13">
@@ -2805,19 +2805,19 @@
       <c r="T13">
         <v>37</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="2">
         <v>21</v>
       </c>
       <c r="V13">
         <v>26</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="2">
         <v>20</v>
       </c>
       <c r="X13">
         <v>37</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="2">
         <v>20</v>
       </c>
       <c r="Z13">
@@ -2909,7 +2909,7 @@
       <c r="N14" s="2">
         <v>14</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="2">
         <v>17</v>
       </c>
       <c r="P14">
@@ -2921,10 +2921,10 @@
       <c r="R14">
         <v>27</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="2">
         <v>17</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="2">
         <v>19</v>
       </c>
       <c r="U14">
@@ -2933,7 +2933,7 @@
       <c r="V14">
         <v>30</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="2">
         <v>19</v>
       </c>
       <c r="X14">
@@ -2951,7 +2951,7 @@
       <c r="AB14">
         <v>34</v>
       </c>
-      <c r="AC14">
+      <c r="AC14" s="2">
         <v>21</v>
       </c>
       <c r="AD14">
@@ -3004,13 +3004,13 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>18</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>17</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>17</v>
       </c>
       <c r="E15">
@@ -3025,19 +3025,19 @@
       <c r="H15">
         <v>22</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="2">
         <v>18</v>
       </c>
       <c r="J15">
         <v>31</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="2">
         <v>19</v>
       </c>
       <c r="L15">
         <v>23</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="2">
         <v>16</v>
       </c>
       <c r="N15">
@@ -3046,13 +3046,13 @@
       <c r="O15" s="2">
         <v>14</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="2">
         <v>19</v>
       </c>
       <c r="Q15" s="2">
         <v>14</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="2">
         <v>19</v>
       </c>
       <c r="S15">
@@ -3064,13 +3064,13 @@
       <c r="U15">
         <v>37</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="2">
         <v>20</v>
       </c>
       <c r="W15" s="2">
         <v>12</v>
       </c>
-      <c r="X15">
+      <c r="X15" s="2">
         <v>21</v>
       </c>
       <c r="Y15">
@@ -3094,7 +3094,7 @@
       <c r="AE15">
         <v>27</v>
       </c>
-      <c r="AF15">
+      <c r="AF15" s="2">
         <v>21</v>
       </c>
       <c r="AG15">
@@ -3171,7 +3171,7 @@
       <c r="E16">
         <v>24</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>17</v>
       </c>
       <c r="G16">
@@ -3183,7 +3183,7 @@
       <c r="I16">
         <v>36</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="2">
         <v>15</v>
       </c>
       <c r="K16">
@@ -3239,25 +3239,25 @@
       <c r="B17" s="5">
         <v>11</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>20</v>
       </c>
       <c r="D17">
         <v>38</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>17</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>19</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>19</v>
       </c>
       <c r="H17">
         <v>72</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="2">
         <v>18</v>
       </c>
       <c r="J17">
@@ -3328,10 +3328,10 @@
       <c r="C18">
         <v>23</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>15</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>17</v>
       </c>
       <c r="F18" s="2">
@@ -3343,7 +3343,7 @@
       <c r="H18" s="2">
         <v>10</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="2">
         <v>17</v>
       </c>
       <c r="J18">
@@ -3352,7 +3352,7 @@
       <c r="K18">
         <v>3</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="2">
         <v>17</v>
       </c>
       <c r="M18">
@@ -3361,7 +3361,7 @@
       <c r="N18">
         <v>30</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="2">
         <v>16</v>
       </c>
       <c r="P18">
@@ -3426,7 +3426,7 @@
       <c r="D19">
         <v>26</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>21</v>
       </c>
       <c r="F19">
@@ -3435,7 +3435,7 @@
       <c r="G19">
         <v>30</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="2">
         <v>21</v>
       </c>
       <c r="I19">
@@ -3447,7 +3447,7 @@
       <c r="K19">
         <v>22</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="2">
         <v>20</v>
       </c>
       <c r="M19">
@@ -3465,10 +3465,10 @@
       <c r="Q19">
         <v>22</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="2">
         <v>16</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="2">
         <v>21</v>
       </c>
       <c r="T19">
@@ -3483,7 +3483,7 @@
       <c r="W19">
         <v>30</v>
       </c>
-      <c r="X19">
+      <c r="X19" s="2">
         <v>17</v>
       </c>
       <c r="Y19">
@@ -3495,7 +3495,7 @@
       <c r="AA19" s="2">
         <v>14</v>
       </c>
-      <c r="AB19">
+      <c r="AB19" s="2">
         <v>21</v>
       </c>
       <c r="AC19">
@@ -3519,7 +3519,7 @@
       <c r="AI19">
         <v>37</v>
       </c>
-      <c r="AJ19">
+      <c r="AJ19" s="2">
         <v>16</v>
       </c>
       <c r="AK19">
@@ -3540,7 +3540,7 @@
       <c r="AP19">
         <v>26</v>
       </c>
-      <c r="AQ19">
+      <c r="AQ19" s="2">
         <v>17</v>
       </c>
     </row>
@@ -3566,16 +3566,16 @@
       <c r="G20" s="2">
         <v>11</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="2">
         <v>18</v>
       </c>
       <c r="I20" s="2">
         <v>10</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="2">
         <v>21</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="2">
         <v>18</v>
       </c>
       <c r="L20">
@@ -3596,13 +3596,13 @@
       <c r="Q20" s="2">
         <v>11</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="2">
         <v>15</v>
       </c>
       <c r="S20">
         <v>51</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="2">
         <v>15</v>
       </c>
       <c r="U20" s="4">
@@ -3665,7 +3665,7 @@
       <c r="AN20" s="2">
         <v>14</v>
       </c>
-      <c r="AO20">
+      <c r="AO20" s="2">
         <v>18</v>
       </c>
       <c r="AP20" s="2">
@@ -3680,7 +3680,7 @@
       <c r="AS20">
         <v>27</v>
       </c>
-      <c r="AT20">
+      <c r="AT20" s="2">
         <v>18</v>
       </c>
       <c r="AU20" s="2">
@@ -3689,10 +3689,10 @@
       <c r="AV20" s="2">
         <v>10</v>
       </c>
-      <c r="AW20">
+      <c r="AW20" s="2">
         <v>15</v>
       </c>
-      <c r="AX20">
+      <c r="AX20" s="2">
         <v>21</v>
       </c>
       <c r="AY20">
@@ -3703,7 +3703,7 @@
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>21</v>
       </c>
       <c r="C21" s="2">
@@ -3727,7 +3727,7 @@
       <c r="I21" s="2">
         <v>12</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="2">
         <v>18</v>
       </c>
       <c r="K21" s="2">
@@ -3748,7 +3748,7 @@
       <c r="P21" s="2">
         <v>14</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="2">
         <v>20</v>
       </c>
       <c r="R21">
@@ -3766,7 +3766,7 @@
       <c r="V21">
         <v>24</v>
       </c>
-      <c r="W21">
+      <c r="W21" s="2">
         <v>20</v>
       </c>
       <c r="X21">
@@ -3781,7 +3781,7 @@
       <c r="AA21" s="2">
         <v>13</v>
       </c>
-      <c r="AB21">
+      <c r="AB21" s="2">
         <v>21</v>
       </c>
       <c r="AC21">
@@ -3790,16 +3790,16 @@
       <c r="AD21" s="2">
         <v>13</v>
       </c>
-      <c r="AE21">
+      <c r="AE21" s="2">
         <v>20</v>
       </c>
-      <c r="AF21">
+      <c r="AF21" s="2">
         <v>17</v>
       </c>
       <c r="AG21">
         <v>8</v>
       </c>
-      <c r="AH21">
+      <c r="AH21" s="2">
         <v>19</v>
       </c>
       <c r="AI21" s="2">
@@ -3808,25 +3808,25 @@
       <c r="AJ21" s="2">
         <v>14</v>
       </c>
-      <c r="AK21">
+      <c r="AK21" s="2">
         <v>17</v>
       </c>
       <c r="AL21">
         <v>7</v>
       </c>
-      <c r="AM21">
+      <c r="AM21" s="2">
         <v>19</v>
       </c>
       <c r="AN21">
         <v>53</v>
       </c>
-      <c r="AO21">
+      <c r="AO21" s="2">
         <v>17</v>
       </c>
-      <c r="AP21">
+      <c r="AP21" s="2">
         <v>16</v>
       </c>
-      <c r="AQ21">
+      <c r="AQ21" s="2">
         <v>16</v>
       </c>
       <c r="AR21">
@@ -3900,10 +3900,10 @@
       <c r="O22">
         <v>8</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="2">
         <v>18</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="2">
         <v>19</v>
       </c>
       <c r="R22">
@@ -3951,7 +3951,7 @@
       <c r="AF22">
         <v>3</v>
       </c>
-      <c r="AG22">
+      <c r="AG22" s="2">
         <v>18</v>
       </c>
       <c r="AH22">
@@ -3960,7 +3960,7 @@
       <c r="AI22">
         <v>3</v>
       </c>
-      <c r="AJ22">
+      <c r="AJ22" s="2">
         <v>21</v>
       </c>
       <c r="AK22">
@@ -3987,16 +3987,16 @@
       <c r="AR22" s="2">
         <v>12</v>
       </c>
-      <c r="AS22">
+      <c r="AS22" s="2">
         <v>15</v>
       </c>
-      <c r="AT22">
+      <c r="AT22" s="2">
         <v>21</v>
       </c>
       <c r="AU22" s="2">
         <v>10</v>
       </c>
-      <c r="AV22">
+      <c r="AV22" s="2">
         <v>20</v>
       </c>
       <c r="AW22" s="2">
@@ -4037,7 +4037,7 @@
       <c r="I23">
         <v>36</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="2">
         <v>18</v>
       </c>
       <c r="K23">
@@ -4111,7 +4111,7 @@
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>18</v>
       </c>
       <c r="C24">
@@ -4120,10 +4120,10 @@
       <c r="D24">
         <v>22</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>17</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>19</v>
       </c>
       <c r="G24" s="2">
@@ -4132,13 +4132,13 @@
       <c r="H24">
         <v>29</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="2">
         <v>17</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="2">
         <v>18</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="2">
         <v>20</v>
       </c>
       <c r="L24" s="2">
@@ -4152,19 +4152,19 @@
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>17</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>17</v>
       </c>
       <c r="D25" s="2">
         <v>11</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>16</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>16</v>
       </c>
       <c r="G25" s="2">
@@ -4205,13 +4205,13 @@
       <c r="I26">
         <v>23</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="2">
         <v>20</v>
       </c>
       <c r="K26">
         <v>34</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="2">
         <v>16</v>
       </c>
       <c r="M26">
@@ -4241,13 +4241,13 @@
       <c r="U26">
         <v>6</v>
       </c>
-      <c r="V26">
+      <c r="V26" s="2">
         <v>17</v>
       </c>
       <c r="W26">
         <v>25</v>
       </c>
-      <c r="X26">
+      <c r="X26" s="2">
         <v>18</v>
       </c>
       <c r="Y26">
@@ -4256,7 +4256,7 @@
       <c r="Z26" s="2">
         <v>12</v>
       </c>
-      <c r="AA26">
+      <c r="AA26" s="2">
         <v>21</v>
       </c>
       <c r="AB26" s="2">
@@ -4274,13 +4274,13 @@
       <c r="AF26" s="2">
         <v>9</v>
       </c>
-      <c r="AG26">
+      <c r="AG26" s="2">
         <v>20</v>
       </c>
       <c r="AH26">
         <v>24</v>
       </c>
-      <c r="AI26">
+      <c r="AI26" s="2">
         <v>17</v>
       </c>
       <c r="AJ26" s="2">
@@ -4319,7 +4319,7 @@
       <c r="AU26" s="2">
         <v>13</v>
       </c>
-      <c r="AV26">
+      <c r="AV26" s="2">
         <v>15</v>
       </c>
       <c r="AW26">
@@ -4334,13 +4334,13 @@
       <c r="AZ26">
         <v>23</v>
       </c>
-      <c r="BA26">
+      <c r="BA26" s="2">
         <v>15</v>
       </c>
       <c r="BB26" s="2">
         <v>12</v>
       </c>
-      <c r="BC26">
+      <c r="BC26" s="2">
         <v>17</v>
       </c>
       <c r="BD26" s="2">
@@ -4349,13 +4349,13 @@
       <c r="BE26" s="2">
         <v>12</v>
       </c>
-      <c r="BF26">
+      <c r="BF26" s="2">
         <v>21</v>
       </c>
       <c r="BG26" s="2">
         <v>14</v>
       </c>
-      <c r="BH26">
+      <c r="BH26" s="2">
         <v>21</v>
       </c>
       <c r="BI26">
@@ -4367,7 +4367,7 @@
       <c r="BK26" s="2">
         <v>12</v>
       </c>
-      <c r="BL26">
+      <c r="BL26" s="2">
         <v>19</v>
       </c>
       <c r="BM26" s="2">
@@ -4384,7 +4384,7 @@
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>19</v>
       </c>
       <c r="C27">
@@ -4417,7 +4417,7 @@
       <c r="L27">
         <v>23</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="2">
         <v>17</v>
       </c>
       <c r="N27">
@@ -4426,10 +4426,10 @@
       <c r="O27">
         <v>22</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="2">
         <v>21</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="2">
         <v>21</v>
       </c>
       <c r="R27">
@@ -4438,10 +4438,10 @@
       <c r="S27">
         <v>23</v>
       </c>
-      <c r="T27">
+      <c r="T27" s="2">
         <v>15</v>
       </c>
-      <c r="U27">
+      <c r="U27" s="2">
         <v>18</v>
       </c>
       <c r="V27" s="2">
@@ -4465,7 +4465,7 @@
       <c r="AB27">
         <v>22</v>
       </c>
-      <c r="AC27">
+      <c r="AC27" s="2">
         <v>17</v>
       </c>
       <c r="AD27">
@@ -4486,25 +4486,25 @@
       <c r="AI27">
         <v>22</v>
       </c>
-      <c r="AJ27">
+      <c r="AJ27" s="2">
         <v>19</v>
       </c>
       <c r="AK27">
         <v>32</v>
       </c>
-      <c r="AL27">
+      <c r="AL27" s="2">
         <v>21</v>
       </c>
       <c r="AM27">
         <v>28</v>
       </c>
-      <c r="AN27">
+      <c r="AN27" s="2">
         <v>18</v>
       </c>
-      <c r="AO27">
+      <c r="AO27" s="2">
         <v>16</v>
       </c>
-      <c r="AP27">
+      <c r="AP27" s="2">
         <v>18</v>
       </c>
       <c r="AQ27">
@@ -4574,10 +4574,10 @@
       <c r="D29">
         <v>27</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>17</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>17</v>
       </c>
       <c r="G29" s="2">
@@ -4586,7 +4586,7 @@
       <c r="H29">
         <v>27</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="2">
         <v>18</v>
       </c>
       <c r="J29" s="2">
@@ -4637,10 +4637,10 @@
       <c r="Y29">
         <v>27</v>
       </c>
-      <c r="Z29">
+      <c r="Z29" s="2">
         <v>17</v>
       </c>
-      <c r="AA29">
+      <c r="AA29" s="2">
         <v>21</v>
       </c>
       <c r="AB29">
@@ -4649,13 +4649,13 @@
       <c r="AC29">
         <v>26</v>
       </c>
-      <c r="AD29">
+      <c r="AD29" s="2">
         <v>21</v>
       </c>
       <c r="AE29">
         <v>26</v>
       </c>
-      <c r="AF29">
+      <c r="AF29" s="2">
         <v>18</v>
       </c>
       <c r="AG29">
@@ -4667,7 +4667,7 @@
       <c r="AI29">
         <v>31</v>
       </c>
-      <c r="AJ29">
+      <c r="AJ29" s="2">
         <v>15</v>
       </c>
       <c r="AK29">
@@ -4688,7 +4688,7 @@
       <c r="AP29">
         <v>26</v>
       </c>
-      <c r="AQ29">
+      <c r="AQ29" s="2">
         <v>20</v>
       </c>
       <c r="AR29">
@@ -4714,7 +4714,7 @@
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>21</v>
       </c>
       <c r="C30">
@@ -4741,7 +4741,7 @@
       <c r="J30">
         <v>27</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="2">
         <v>21</v>
       </c>
       <c r="L30">
@@ -4770,34 +4770,34 @@
       <c r="D31">
         <v>5</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>19</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>15</v>
       </c>
       <c r="G31" s="2">
         <v>11</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="2">
         <v>16</v>
       </c>
       <c r="I31" s="2">
         <v>14</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="2">
         <v>17</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="2">
         <v>15</v>
       </c>
       <c r="L31" s="2">
         <v>11</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="2">
         <v>15</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="2">
         <v>15</v>
       </c>
       <c r="O31" s="2">
@@ -4808,7 +4808,7 @@
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>20</v>
       </c>
       <c r="C32">
@@ -4817,7 +4817,7 @@
       <c r="D32">
         <v>5</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>21</v>
       </c>
     </row>
@@ -4825,13 +4825,13 @@
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>15</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>16</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>15</v>
       </c>
       <c r="E33" s="2">
@@ -4843,13 +4843,13 @@
       <c r="G33" s="2">
         <v>14</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="2">
         <v>17</v>
       </c>
       <c r="I33" s="2">
         <v>14</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="2">
         <v>15</v>
       </c>
     </row>
@@ -4857,7 +4857,7 @@
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <v>21</v>
       </c>
     </row>
@@ -4865,7 +4865,7 @@
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <v>16</v>
       </c>
       <c r="C35" s="2">
@@ -4882,7 +4882,7 @@
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>16</v>
       </c>
       <c r="C36" s="2">
@@ -4897,10 +4897,10 @@
       <c r="F36" s="2">
         <v>14</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="2">
         <v>16</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="2">
         <v>20</v>
       </c>
     </row>
@@ -4914,7 +4914,7 @@
       <c r="C37" s="2">
         <v>14</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
         <v>19</v>
       </c>
     </row>
@@ -4922,13 +4922,13 @@
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="2">
         <v>17</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="2">
         <v>20</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>19</v>
       </c>
     </row>
@@ -4936,13 +4936,13 @@
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="2">
         <v>18</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="2">
         <v>15</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="2">
         <v>20</v>
       </c>
     </row>
@@ -4950,7 +4950,7 @@
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>15</v>
       </c>
       <c r="C40">
@@ -4961,10 +4961,10 @@
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="2">
         <v>17</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="2">
         <v>17</v>
       </c>
       <c r="D41" s="2">
@@ -4976,7 +4976,7 @@
       <c r="F41" s="2">
         <v>11</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="2">
         <v>15</v>
       </c>
       <c r="H41" s="2">
@@ -4985,13 +4985,13 @@
       <c r="I41">
         <v>23</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="2">
         <v>17</v>
       </c>
       <c r="K41" s="2">
         <v>12</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="2">
         <v>17</v>
       </c>
       <c r="M41" s="2">
@@ -5000,7 +5000,7 @@
       <c r="N41" s="2">
         <v>9</v>
       </c>
-      <c r="O41">
+      <c r="O41" s="2">
         <v>21</v>
       </c>
     </row>
@@ -5011,7 +5011,7 @@
       <c r="B42" s="2">
         <v>14</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="2">
         <v>17</v>
       </c>
       <c r="D42">
@@ -5028,7 +5028,7 @@
       <c r="C43">
         <v>23</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="2">
         <v>17</v>
       </c>
       <c r="E43">
@@ -5103,7 +5103,7 @@
       <c r="AB43">
         <v>66</v>
       </c>
-      <c r="AC43">
+      <c r="AC43" s="2">
         <v>20</v>
       </c>
     </row>
@@ -5156,7 +5156,7 @@
       <c r="P44">
         <v>47</v>
       </c>
-      <c r="Q44">
+      <c r="Q44" s="2">
         <v>20</v>
       </c>
     </row>
@@ -5324,7 +5324,7 @@
       <c r="F47">
         <v>42</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="2">
         <v>15</v>
       </c>
       <c r="H47">
@@ -5410,7 +5410,7 @@
       <c r="E48">
         <v>25</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="2">
         <v>21</v>
       </c>
       <c r="G48">
@@ -5425,13 +5425,13 @@
       <c r="J48">
         <v>33</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="2">
         <v>21</v>
       </c>
       <c r="L48">
         <v>36</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="2">
         <v>21</v>
       </c>
       <c r="N48" s="2">
@@ -5449,24 +5449,24 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B49">
         <v>31</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="2">
         <v>16</v>
       </c>
       <c r="D49">
         <v>23</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="2">
         <v>21</v>
       </c>
       <c r="F49" s="2">
         <v>13</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="2">
         <v>20</v>
       </c>
       <c r="H49">
@@ -5502,42 +5502,42 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B50">
         <v>24</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="2">
         <v>17</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="2">
         <v>18</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="2">
         <v>18</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="2">
         <v>21</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="2">
         <v>18</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="2">
         <v>16</v>
       </c>
       <c r="I50">
         <v>24</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="2">
         <v>15</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="2">
         <v>18</v>
       </c>
       <c r="L50">
         <v>33</v>
       </c>
-      <c r="M50">
+      <c r="M50" s="2">
         <v>21</v>
       </c>
       <c r="N50" s="2">
@@ -5546,12 +5546,12 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B51">
         <v>24</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="2">
         <v>21</v>
       </c>
       <c r="D51">
@@ -5563,13 +5563,13 @@
       <c r="F51">
         <v>26</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B52">
         <v>23</v>
@@ -5577,7 +5577,7 @@
       <c r="C52">
         <v>22</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="2">
         <v>21</v>
       </c>
       <c r="E52">
@@ -5592,7 +5592,7 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B53">
         <v>30</v>
@@ -5600,7 +5600,7 @@
       <c r="C53">
         <v>30</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="2">
         <v>21</v>
       </c>
       <c r="E53">
@@ -5609,7 +5609,7 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B54">
         <v>29</v>
@@ -5620,24 +5620,24 @@
       <c r="D54">
         <v>25</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B55" s="2">
         <v>10</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="2">
         <v>20</v>
       </c>
       <c r="D55" s="2">
         <v>13</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="2">
         <v>18</v>
       </c>
       <c r="F55">
@@ -5646,52 +5646,52 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B56" s="2">
         <v>12</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="2">
         <v>17</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57">
+        <v>64</v>
+      </c>
+      <c r="B57" s="2">
         <v>20</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="2">
         <v>15</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="2">
         <v>16</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="2">
         <v>16</v>
       </c>
       <c r="F57">
         <v>25</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58">
+        <v>65</v>
+      </c>
+      <c r="B58" s="2">
         <v>18</v>
       </c>
       <c r="C58">
         <v>26</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="2">
         <v>17</v>
       </c>
       <c r="E58">
@@ -5700,21 +5700,21 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59">
+        <v>49</v>
+      </c>
+      <c r="B59" s="2">
         <v>16</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="2">
         <v>15</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="2">
         <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B60">
         <v>25</v>
@@ -5722,24 +5722,24 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B61" s="2">
         <v>14</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="2">
         <v>18</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="2">
         <v>19</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="2">
         <v>16</v>
       </c>
       <c r="F61" s="2">
         <v>14</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="2">
         <v>20</v>
       </c>
       <c r="H61">
@@ -5766,7 +5766,7 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B62">
         <v>27</v>
@@ -5774,10 +5774,10 @@
       <c r="C62">
         <v>26</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="2">
         <v>18</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="2">
         <v>17</v>
       </c>
       <c r="F62" s="2">
@@ -5786,7 +5786,7 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B63">
         <v>25</v>
@@ -5797,7 +5797,7 @@
       <c r="D63">
         <v>22</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="2">
         <v>19</v>
       </c>
       <c r="F63" s="2">
@@ -5806,22 +5806,22 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64">
+        <v>52</v>
+      </c>
+      <c r="B64" s="2">
         <v>21</v>
       </c>
       <c r="C64">
         <v>22</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="2">
         <v>18</v>
       </c>
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B65" s="2">
         <v>10</v>
@@ -5832,7 +5832,7 @@
       <c r="D65">
         <v>24</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="2">
         <v>21</v>
       </c>
       <c r="F65" s="2">
@@ -5841,7 +5841,7 @@
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B66" s="2">
         <v>13</v>
@@ -5850,16 +5850,16 @@
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67">
+        <v>55</v>
+      </c>
+      <c r="B67" s="2">
         <v>15</v>
       </c>
       <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B68">
         <v>25</v>
@@ -5868,9 +5868,9 @@
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2">
         <v>20</v>
       </c>
       <c r="C69">
@@ -5885,55 +5885,55 @@
       <c r="F69" s="2">
         <v>14</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="2">
         <v>17</v>
       </c>
-      <c r="H69">
+      <c r="H69" s="2">
         <v>17</v>
       </c>
       <c r="I69" s="2">
         <v>13</v>
       </c>
-      <c r="J69">
+      <c r="J69" s="2">
         <v>21</v>
       </c>
       <c r="K69" s="2">
         <v>11</v>
       </c>
-      <c r="L69">
+      <c r="L69" s="2">
         <v>19</v>
       </c>
-      <c r="M69">
+      <c r="M69" s="2">
         <v>17</v>
       </c>
-      <c r="N69">
+      <c r="N69" s="2">
         <v>18</v>
       </c>
-      <c r="O69">
+      <c r="O69" s="2">
         <v>20</v>
       </c>
       <c r="P69">
         <v>8</v>
       </c>
-      <c r="Q69">
+      <c r="Q69" s="2">
         <v>21</v>
       </c>
-      <c r="R69">
+      <c r="R69" s="2">
         <v>18</v>
       </c>
       <c r="S69">
         <v>24</v>
       </c>
-      <c r="T69">
+      <c r="T69" s="2">
         <v>21</v>
       </c>
-      <c r="U69">
+      <c r="U69" s="2">
         <v>15</v>
       </c>
       <c r="V69">
         <v>27</v>
       </c>
-      <c r="W69">
+      <c r="W69" s="2">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished verse 33; Isaiah 33 was missing up to verse 11, so I fixed it
</commit_message>
<xml_diff>
--- a/ref/Bible_data_ch_verses.xlsx
+++ b/ref/Bible_data_ch_verses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E4E9E840-0423-4022-A8D3-939612B00AC4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{47CF5EF7-689E-4558-91B8-F321C1D40FA5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1085,7 +1085,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R14" sqref="R14"/>
+      <selection pane="bottomRight" activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
finished verse 35; fixed Catholic OT discrepancies with the KJV OT; I only checked the number of chapters for all books, but not the number of verses in every chapter
</commit_message>
<xml_diff>
--- a/ref/Bible_data_ch_verses.xlsx
+++ b/ref/Bible_data_ch_verses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{47CF5EF7-689E-4558-91B8-F321C1D40FA5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9F358D5C-5A41-48A2-A58B-F9737A792E61}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1082,10 +1082,10 @@
   <dimension ref="A1:BO69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z22" sqref="Z22"/>
+      <selection pane="bottomRight" activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3345,24 +3345,6 @@
       <c r="K18" s="1">
         <v>3</v>
       </c>
-      <c r="L18" s="1">
-        <v>17</v>
-      </c>
-      <c r="M18" s="1">
-        <v>8</v>
-      </c>
-      <c r="N18" s="1">
-        <v>30</v>
-      </c>
-      <c r="O18" s="1">
-        <v>16</v>
-      </c>
-      <c r="P18" s="1">
-        <v>24</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>10</v>
-      </c>
       <c r="AL18" s="1" t="s">
         <v>3</v>
       </c>
@@ -4714,13 +4696,13 @@
         <v>49</v>
       </c>
       <c r="D30" s="1">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="E30" s="1">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F30" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G30" s="1">
         <v>29</v>
@@ -4742,12 +4724,6 @@
       </c>
       <c r="M30" s="1">
         <v>13</v>
-      </c>
-      <c r="N30" s="1">
-        <v>64</v>
-      </c>
-      <c r="O30" s="1">
-        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:67" x14ac:dyDescent="0.25">
@@ -4805,12 +4781,9 @@
         <v>20</v>
       </c>
       <c r="C32" s="1">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D32" s="1">
-        <v>5</v>
-      </c>
-      <c r="E32" s="1">
         <v>21</v>
       </c>
     </row>
@@ -5008,7 +4981,10 @@
         <v>17</v>
       </c>
       <c r="D42" s="1">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="E42" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
verses 37 - 56 completed
</commit_message>
<xml_diff>
--- a/ref/Bible_data_ch_verses.xlsx
+++ b/ref/Bible_data_ch_verses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8617C02F-B4F3-4C86-A0E2-A7A305327DAB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E893C5-3461-44E4-8D18-40A390D38040}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="70">
   <si>
     <t>Book Name</t>
   </si>
@@ -236,7 +236,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,8 +377,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,12 +565,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -725,13 +726,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1090,10 +1090,10 @@
   <dimension ref="A1:BO69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE31" sqref="AE31"/>
+      <selection pane="bottomRight" activeCell="BD1" sqref="BD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1213,7 @@
       <c r="AI1" s="2">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4">
+      <c r="AJ1" s="2">
         <v>35</v>
       </c>
       <c r="AK1" s="2">
@@ -1264,7 +1264,7 @@
       <c r="AZ1" s="2">
         <v>51</v>
       </c>
-      <c r="BA1" s="2">
+      <c r="BA1" s="4">
         <v>52</v>
       </c>
       <c r="BB1" s="2">
@@ -1389,7 +1389,7 @@
       <c r="Z2" s="1">
         <v>34</v>
       </c>
-      <c r="AA2" s="5">
+      <c r="AA2" s="1">
         <v>35</v>
       </c>
       <c r="AB2" s="1">
@@ -1398,7 +1398,7 @@
       <c r="AC2" s="1">
         <v>22</v>
       </c>
-      <c r="AD2" s="5">
+      <c r="AD2" s="1">
         <v>35</v>
       </c>
       <c r="AE2" s="1">
@@ -1493,7 +1493,7 @@
       <c r="I3" s="1">
         <v>28</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="1">
         <v>35</v>
       </c>
       <c r="K3" s="1">
@@ -1562,16 +1562,16 @@
       <c r="AF3" s="1">
         <v>18</v>
       </c>
-      <c r="AG3" s="5">
+      <c r="AG3" s="1">
         <v>35</v>
       </c>
       <c r="AH3" s="1">
         <v>23</v>
       </c>
-      <c r="AI3" s="5">
+      <c r="AI3" s="1">
         <v>35</v>
       </c>
-      <c r="AJ3" s="5">
+      <c r="AJ3" s="1">
         <v>35</v>
       </c>
       <c r="AK3" s="1">
@@ -1633,7 +1633,7 @@
       <c r="D4" s="1">
         <v>17</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="1">
         <v>35</v>
       </c>
       <c r="F4" s="1">
@@ -1809,7 +1809,7 @@
       <c r="K5" s="1">
         <v>36</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="1">
         <v>35</v>
       </c>
       <c r="M5" s="1">
@@ -1824,7 +1824,7 @@
       <c r="P5" s="1">
         <v>41</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="1">
         <v>35</v>
       </c>
       <c r="R5" s="1">
@@ -1839,7 +1839,7 @@
       <c r="U5" s="1">
         <v>29</v>
       </c>
-      <c r="V5" s="5">
+      <c r="V5" s="1">
         <v>35</v>
       </c>
       <c r="W5" s="1">
@@ -2027,7 +2027,7 @@
       <c r="AF6" s="1">
         <v>30</v>
       </c>
-      <c r="AG6" s="1">
+      <c r="AG6" s="3">
         <v>52</v>
       </c>
       <c r="AH6" s="1">
@@ -2110,7 +2110,7 @@
       <c r="H7" s="1">
         <v>26</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="1">
         <v>35</v>
       </c>
       <c r="J7" s="1">
@@ -2229,7 +2229,7 @@
       <c r="H8" s="1">
         <v>25</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="1">
         <v>35</v>
       </c>
       <c r="J8" s="1">
@@ -2416,10 +2416,10 @@
       <c r="N10" s="1">
         <v>23</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="3">
         <v>52</v>
       </c>
-      <c r="P10" s="5">
+      <c r="P10" s="1">
         <v>35</v>
       </c>
       <c r="Q10" s="1">
@@ -3424,7 +3424,7 @@
       <c r="I19" s="1">
         <v>22</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="1">
         <v>35</v>
       </c>
       <c r="K19" s="1">
@@ -3442,7 +3442,7 @@
       <c r="O19" s="1">
         <v>22</v>
       </c>
-      <c r="P19" s="5">
+      <c r="P19" s="1">
         <v>35</v>
       </c>
       <c r="Q19" s="1">
@@ -3850,7 +3850,7 @@
       <c r="D22" s="1">
         <v>22</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="1">
         <v>35</v>
       </c>
       <c r="F22" s="1">
@@ -4002,7 +4002,7 @@
       <c r="C23" s="1">
         <v>22</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="1">
         <v>35</v>
       </c>
       <c r="E23" s="1">
@@ -4011,7 +4011,7 @@
       <c r="F23" s="1">
         <v>23</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="1">
         <v>35</v>
       </c>
       <c r="H23" s="1">
@@ -4035,7 +4035,7 @@
       <c r="N23" s="1">
         <v>25</v>
       </c>
-      <c r="O23" s="5">
+      <c r="O23" s="1">
         <v>35</v>
       </c>
       <c r="P23" s="1">
@@ -4062,7 +4062,7 @@
       <c r="W23" s="1">
         <v>29</v>
       </c>
-      <c r="X23" s="5">
+      <c r="X23" s="1">
         <v>35</v>
       </c>
       <c r="Y23" s="1">
@@ -4689,7 +4689,7 @@
       <c r="AV29" s="1">
         <v>23</v>
       </c>
-      <c r="AW29" s="5">
+      <c r="AW29" s="1">
         <v>35</v>
       </c>
     </row>
@@ -5050,7 +5050,7 @@
       <c r="R43" s="1">
         <v>27</v>
       </c>
-      <c r="S43" s="5">
+      <c r="S43" s="1">
         <v>35</v>
       </c>
       <c r="T43" s="1">
@@ -5094,7 +5094,7 @@
       <c r="C44" s="1">
         <v>28</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="1">
         <v>35</v>
       </c>
       <c r="E44" s="1">
@@ -5115,7 +5115,7 @@
       <c r="J44" s="1">
         <v>50</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44" s="3">
         <v>52</v>
       </c>
       <c r="L44" s="1">
@@ -5144,7 +5144,7 @@
       <c r="B45" s="1">
         <v>80</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="3">
         <v>52</v>
       </c>
       <c r="D45" s="1">
@@ -5177,10 +5177,10 @@
       <c r="M45" s="1">
         <v>59</v>
       </c>
-      <c r="N45" s="5">
+      <c r="N45" s="1">
         <v>35</v>
       </c>
-      <c r="O45" s="5">
+      <c r="O45" s="1">
         <v>35</v>
       </c>
       <c r="P45" s="1">
@@ -5322,7 +5322,7 @@
       <c r="M47" s="1">
         <v>25</v>
       </c>
-      <c r="N47" s="1">
+      <c r="N47" s="3">
         <v>52</v>
       </c>
       <c r="O47" s="1">
@@ -5352,7 +5352,7 @@
       <c r="W47" s="1">
         <v>30</v>
       </c>
-      <c r="X47" s="5">
+      <c r="X47" s="1">
         <v>35</v>
       </c>
       <c r="Y47" s="1">

</xml_diff>